<commit_message>
Cleaned the code up. Changed the CourseList.addGrade to check iteratively. Changed the output format to resemble the excel more accuratly.
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8B113BA1-1472-42DD-9F19-6C45DBBC98F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="5445" activeTab="1"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="18225" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="4" r:id="rId1"/>
@@ -12,7 +13,8 @@
     <sheet name="Equivelents" sheetId="2" r:id="rId3"/>
     <sheet name="Areas" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A163:S176"/>
 </workbook>
 </file>
 
@@ -754,7 +756,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,6 +807,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -852,7 +857,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -885,9 +890,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -920,6 +942,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1095,10 +1134,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -4853,10 +4892,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F9"/>
     </sheetView>
   </sheetViews>
@@ -5048,7 +5087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
@@ -5299,7 +5338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
started the excel reader
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8B113BA1-1472-42DD-9F19-6C45DBBC98F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{45F633B1-D4DD-4E85-89CF-664C99B51BE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="18225" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18255" windowHeight="12375" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Areas" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A163:S176"/>
+  <oleSize ref="A1:I11"/>
 </workbook>
 </file>
 
@@ -1137,7 +1137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -5341,7 +5341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added name to the transcript object
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{45F633B1-D4DD-4E85-89CF-664C99B51BE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CF25E3E4-0759-4716-A03F-299460BC7354}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18255" windowHeight="12375" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="0" windowWidth="18285" windowHeight="12900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Areas" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:I11"/>
+  <oleSize ref="A1:J11"/>
 </workbook>
 </file>
 
@@ -4895,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5341,8 +5341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changes made during demo
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CF25E3E4-0759-4716-A03F-299460BC7354}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uwesh/Desktop/Team6/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2672CB40-C62B-A242-9F87-5AAC104E8D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="18285" windowHeight="12900" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="18280" windowHeight="12900" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="4" r:id="rId1"/>
@@ -14,12 +19,11 @@
     <sheet name="Areas" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:J11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="205">
   <si>
     <t>course</t>
   </si>
@@ -39,21 +43,6 @@
     <t>exceeds</t>
   </si>
   <si>
-    <t>CMPE2412</t>
-  </si>
-  <si>
-    <t>CMPE3221</t>
-  </si>
-  <si>
-    <t>CMPE3232</t>
-  </si>
-  <si>
-    <t>CMPE4273</t>
-  </si>
-  <si>
-    <t>CMPECOOP</t>
-  </si>
-  <si>
     <t>ECE3031</t>
   </si>
   <si>
@@ -129,13 +118,514 @@
     <t>ECECOOP</t>
   </si>
   <si>
-    <t>EE2711</t>
-  </si>
-  <si>
-    <t>EE2722</t>
-  </si>
-  <si>
-    <t>EE3031</t>
+    <t>ECE2412</t>
+  </si>
+  <si>
+    <t>ECE2711</t>
+  </si>
+  <si>
+    <t>ECE2722</t>
+  </si>
+  <si>
+    <t>CE3963</t>
+  </si>
+  <si>
+    <t>CHEM1982</t>
+  </si>
+  <si>
+    <t>CHEM1987</t>
+  </si>
+  <si>
+    <t>ECE1813</t>
+  </si>
+  <si>
+    <t>ECE2213</t>
+  </si>
+  <si>
+    <t>ADM1015</t>
+  </si>
+  <si>
+    <t>ADM1113</t>
+  </si>
+  <si>
+    <t>ADM2213</t>
+  </si>
+  <si>
+    <t>ADM2223</t>
+  </si>
+  <si>
+    <t>ADM2313</t>
+  </si>
+  <si>
+    <t>ADM2413</t>
+  </si>
+  <si>
+    <t>ADM2513</t>
+  </si>
+  <si>
+    <t>ADM3155</t>
+  </si>
+  <si>
+    <t>ADM3315</t>
+  </si>
+  <si>
+    <t>ADM3415</t>
+  </si>
+  <si>
+    <t>ADM3445</t>
+  </si>
+  <si>
+    <t>ADM4437</t>
+  </si>
+  <si>
+    <t>ANTH1001</t>
+  </si>
+  <si>
+    <t>ANTH1002</t>
+  </si>
+  <si>
+    <t>APSC1013</t>
+  </si>
+  <si>
+    <t>APSC1023</t>
+  </si>
+  <si>
+    <t>APSC2023</t>
+  </si>
+  <si>
+    <t>APSC2028</t>
+  </si>
+  <si>
+    <t>APSC3953</t>
+  </si>
+  <si>
+    <t>BIOL1001</t>
+  </si>
+  <si>
+    <t>BIOL1012</t>
+  </si>
+  <si>
+    <t>BIOL1017</t>
+  </si>
+  <si>
+    <t>BIOL1621</t>
+  </si>
+  <si>
+    <t>BIOL1622</t>
+  </si>
+  <si>
+    <t>BIOL2033</t>
+  </si>
+  <si>
+    <t>BIOL2043</t>
+  </si>
+  <si>
+    <t>BIOL2053</t>
+  </si>
+  <si>
+    <t>BIOL2615</t>
+  </si>
+  <si>
+    <t>BIOL2753</t>
+  </si>
+  <si>
+    <t>BIOL2792</t>
+  </si>
+  <si>
+    <t>CHEM1041</t>
+  </si>
+  <si>
+    <t>CHEM1046</t>
+  </si>
+  <si>
+    <t>CHEM1072</t>
+  </si>
+  <si>
+    <t>CHEM1077</t>
+  </si>
+  <si>
+    <t>CHEM2401</t>
+  </si>
+  <si>
+    <t>CLAS1403</t>
+  </si>
+  <si>
+    <t>CLAS1413</t>
+  </si>
+  <si>
+    <t>CLAS1503</t>
+  </si>
+  <si>
+    <t>CLAS3053</t>
+  </si>
+  <si>
+    <t>CS1003</t>
+  </si>
+  <si>
+    <t>CS1023</t>
+  </si>
+  <si>
+    <t>ECON1001</t>
+  </si>
+  <si>
+    <t>ECON1013</t>
+  </si>
+  <si>
+    <t>ECON1023</t>
+  </si>
+  <si>
+    <t>ECON1073</t>
+  </si>
+  <si>
+    <t>ENGG1003</t>
+  </si>
+  <si>
+    <t>ENGG1015</t>
+  </si>
+  <si>
+    <t>ENGG1082</t>
+  </si>
+  <si>
+    <t>ENGG4013</t>
+  </si>
+  <si>
+    <t>FR1304</t>
+  </si>
+  <si>
+    <t>GEOL1001</t>
+  </si>
+  <si>
+    <t>GEOL1044</t>
+  </si>
+  <si>
+    <t>GEOL1063</t>
+  </si>
+  <si>
+    <t>GEOL1074</t>
+  </si>
+  <si>
+    <t>GER1001</t>
+  </si>
+  <si>
+    <t>GER4023</t>
+  </si>
+  <si>
+    <t>HIST1001</t>
+  </si>
+  <si>
+    <t>HIST3414</t>
+  </si>
+  <si>
+    <t>HIST3925</t>
+  </si>
+  <si>
+    <t>HIST3975</t>
+  </si>
+  <si>
+    <t>HUM1401</t>
+  </si>
+  <si>
+    <t>JPNS1013</t>
+  </si>
+  <si>
+    <t>MATH1003</t>
+  </si>
+  <si>
+    <t>MATH1013</t>
+  </si>
+  <si>
+    <t>MATH1503</t>
+  </si>
+  <si>
+    <t>MATH2513</t>
+  </si>
+  <si>
+    <t>MATH3503</t>
+  </si>
+  <si>
+    <t>PHIL1053</t>
+  </si>
+  <si>
+    <t>PHIL1101</t>
+  </si>
+  <si>
+    <t>PHYS5993</t>
+  </si>
+  <si>
+    <t>POLS1201</t>
+  </si>
+  <si>
+    <t>POLS1203</t>
+  </si>
+  <si>
+    <t>POLS1301</t>
+  </si>
+  <si>
+    <t>POLS1603</t>
+  </si>
+  <si>
+    <t>PSYC1003</t>
+  </si>
+  <si>
+    <t>PSYC1013</t>
+  </si>
+  <si>
+    <t>PSYC1023</t>
+  </si>
+  <si>
+    <t>RCLP1042</t>
+  </si>
+  <si>
+    <t>RUSS1013</t>
+  </si>
+  <si>
+    <t>SE1001</t>
+  </si>
+  <si>
+    <t>SEP1001</t>
+  </si>
+  <si>
+    <t>SOCI1001</t>
+  </si>
+  <si>
+    <t>SOCI1503</t>
+  </si>
+  <si>
+    <t>SOCI1523</t>
+  </si>
+  <si>
+    <t>SOCI1583</t>
+  </si>
+  <si>
+    <t>SOCI2533</t>
+  </si>
+  <si>
+    <t>SOCI2534</t>
+  </si>
+  <si>
+    <t>SPAN1203</t>
+  </si>
+  <si>
+    <t>STAT2593</t>
+  </si>
+  <si>
+    <t>STS1003</t>
+  </si>
+  <si>
+    <t>TME1001</t>
+  </si>
+  <si>
+    <t>TME3013</t>
+  </si>
+  <si>
+    <t>TME3113</t>
+  </si>
+  <si>
+    <t>TME3213</t>
+  </si>
+  <si>
+    <t>TME3313</t>
+  </si>
+  <si>
+    <t>TME3346</t>
+  </si>
+  <si>
+    <t>TME3413</t>
+  </si>
+  <si>
+    <t>TME5025</t>
+  </si>
+  <si>
+    <t>WLCS1002</t>
+  </si>
+  <si>
+    <t>MATH</t>
+  </si>
+  <si>
+    <t>SCIENCE</t>
+  </si>
+  <si>
+    <t>FUNDAMENTALS</t>
+  </si>
+  <si>
+    <t>SPECIALIZED</t>
+  </si>
+  <si>
+    <t>TERMINAL</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>CSE</t>
+  </si>
+  <si>
+    <t>AESL1011</t>
+  </si>
+  <si>
+    <t>CHE2501</t>
+  </si>
+  <si>
+    <t>CHE2506</t>
+  </si>
+  <si>
+    <t>CS1073</t>
+  </si>
+  <si>
+    <t>CS1083</t>
+  </si>
+  <si>
+    <t>CS1203</t>
+  </si>
+  <si>
+    <t>CS3383</t>
+  </si>
+  <si>
+    <t>CS3413</t>
+  </si>
+  <si>
+    <t>CS3853</t>
+  </si>
+  <si>
+    <t>CS6895</t>
+  </si>
+  <si>
+    <t>ECE4143</t>
+  </si>
+  <si>
+    <t>ECE4253</t>
+  </si>
+  <si>
+    <t>ECE4261</t>
+  </si>
+  <si>
+    <t>ECE4323</t>
+  </si>
+  <si>
+    <t>ECE4333</t>
+  </si>
+  <si>
+    <t>ECE4923</t>
+  </si>
+  <si>
+    <t>ECE4933</t>
+  </si>
+  <si>
+    <t>EE6013</t>
+  </si>
+  <si>
+    <t>EE6463</t>
+  </si>
+  <si>
+    <t>EE6513</t>
+  </si>
+  <si>
+    <t>EE6603</t>
+  </si>
+  <si>
+    <t>EE6653</t>
+  </si>
+  <si>
+    <t>EE6997</t>
+  </si>
+  <si>
+    <t>ENGG1001</t>
+  </si>
+  <si>
+    <t>ENGG1013</t>
+  </si>
+  <si>
+    <t>ENGL1500</t>
+  </si>
+  <si>
+    <t>ENVS2023</t>
+  </si>
+  <si>
+    <t>ESCI1012</t>
+  </si>
+  <si>
+    <t>ESL1301</t>
+  </si>
+  <si>
+    <t>ESL1302</t>
+  </si>
+  <si>
+    <t>ESL1303</t>
+  </si>
+  <si>
+    <t>KIN2603</t>
+  </si>
+  <si>
+    <t>KIN3061</t>
+  </si>
+  <si>
+    <t>MAAC3065</t>
+  </si>
+  <si>
+    <t>MATH0863</t>
+  </si>
+  <si>
+    <t>MATH1053</t>
+  </si>
+  <si>
+    <t>MATH1063</t>
+  </si>
+  <si>
+    <t>MATH1863</t>
+  </si>
+  <si>
+    <t>MATH2903</t>
+  </si>
+  <si>
+    <t>MATH3003</t>
+  </si>
+  <si>
+    <t>MATH3213</t>
+  </si>
+  <si>
+    <t>MATH3243</t>
+  </si>
+  <si>
+    <t>MATH3343</t>
+  </si>
+  <si>
+    <t>MATH3543</t>
+  </si>
+  <si>
+    <t>ME1312</t>
+  </si>
+  <si>
+    <t>ME2111</t>
+  </si>
+  <si>
+    <t>ME2122</t>
+  </si>
+  <si>
+    <t>ME2125</t>
+  </si>
+  <si>
+    <t>ME2143</t>
+  </si>
+  <si>
+    <t>ME2145</t>
+  </si>
+  <si>
+    <t>ME3413</t>
+  </si>
+  <si>
+    <t>ME3415</t>
+  </si>
+  <si>
+    <t>PHYS1000</t>
+  </si>
+  <si>
+    <t>PHYS1081</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>SOCIETY</t>
   </si>
   <si>
     <t>EE3111</t>
@@ -144,613 +634,10 @@
     <t>EE3122</t>
   </si>
   <si>
-    <t>EE3312</t>
-  </si>
-  <si>
-    <t>EE3511</t>
-  </si>
-  <si>
-    <t>EE3612</t>
-  </si>
-  <si>
-    <t>EE3821</t>
-  </si>
-  <si>
-    <t>EE3832</t>
-  </si>
-  <si>
-    <t>EECOOP</t>
-  </si>
-  <si>
-    <t>ENGG4025</t>
-  </si>
-  <si>
-    <t>ECE2412</t>
-  </si>
-  <si>
-    <t>ECE2701</t>
-  </si>
-  <si>
-    <t>ECE2711</t>
-  </si>
-  <si>
-    <t>ECE2722</t>
-  </si>
-  <si>
-    <t>EE2703</t>
-  </si>
-  <si>
-    <t>CMPE3242</t>
-  </si>
-  <si>
-    <t>CMPE3812</t>
-  </si>
-  <si>
-    <t>EE4133</t>
-  </si>
-  <si>
-    <t>CMPE4251</t>
-  </si>
-  <si>
-    <t>CMPE4433</t>
-  </si>
-  <si>
-    <t>EE4523</t>
-  </si>
-  <si>
-    <t>EE4531</t>
-  </si>
-  <si>
-    <t>EE4633</t>
-  </si>
-  <si>
-    <t>EE4643</t>
-  </si>
-  <si>
-    <t>CMPE4823</t>
-  </si>
-  <si>
-    <t>CMPE4833</t>
-  </si>
-  <si>
-    <t>EE4913</t>
-  </si>
-  <si>
-    <t>EE2773</t>
-  </si>
-  <si>
-    <t>TME4025</t>
-  </si>
-  <si>
-    <t>EE4833</t>
-  </si>
-  <si>
-    <t>EE4040</t>
-  </si>
-  <si>
-    <t>CECOOP</t>
-  </si>
-  <si>
-    <t>CE3963</t>
-  </si>
-  <si>
-    <t>CHEM1831</t>
-  </si>
-  <si>
-    <t>CHEM1882</t>
-  </si>
-  <si>
-    <t>CHEM1982</t>
-  </si>
-  <si>
-    <t>CHEM1987</t>
-  </si>
-  <si>
-    <t>CMPE2213</t>
-  </si>
-  <si>
-    <t>ECE1813</t>
-  </si>
-  <si>
-    <t>EE1813</t>
-  </si>
-  <si>
-    <t>ME3232</t>
-  </si>
-  <si>
-    <t>ECE2213</t>
-  </si>
-  <si>
-    <t>EE1713</t>
-  </si>
-  <si>
-    <t>EE2213</t>
-  </si>
-  <si>
-    <t>ADM1015</t>
-  </si>
-  <si>
-    <t>ADM1113</t>
-  </si>
-  <si>
-    <t>ADM2213</t>
-  </si>
-  <si>
-    <t>ADM2223</t>
-  </si>
-  <si>
-    <t>ADM2313</t>
-  </si>
-  <si>
-    <t>ADM2413</t>
-  </si>
-  <si>
-    <t>ADM2513</t>
-  </si>
-  <si>
-    <t>ADM3155</t>
-  </si>
-  <si>
-    <t>ADM3315</t>
-  </si>
-  <si>
-    <t>ADM3415</t>
-  </si>
-  <si>
-    <t>ADM3445</t>
-  </si>
-  <si>
-    <t>ADM4437</t>
-  </si>
-  <si>
-    <t>ANTH1001</t>
-  </si>
-  <si>
-    <t>ANTH1002</t>
-  </si>
-  <si>
-    <t>APSC1013</t>
-  </si>
-  <si>
-    <t>APSC1023</t>
-  </si>
-  <si>
-    <t>APSC2023</t>
-  </si>
-  <si>
-    <t>APSC2028</t>
-  </si>
-  <si>
-    <t>APSC3953</t>
-  </si>
-  <si>
-    <t>BIOL1001</t>
-  </si>
-  <si>
-    <t>BIOL1012</t>
-  </si>
-  <si>
-    <t>BIOL1017</t>
-  </si>
-  <si>
-    <t>BIOL1621</t>
-  </si>
-  <si>
-    <t>BIOL1622</t>
-  </si>
-  <si>
-    <t>BIOL2033</t>
-  </si>
-  <si>
-    <t>BIOL2043</t>
-  </si>
-  <si>
-    <t>BIOL2053</t>
-  </si>
-  <si>
-    <t>BIOL2615</t>
-  </si>
-  <si>
-    <t>BIOL2753</t>
-  </si>
-  <si>
-    <t>BIOL2792</t>
-  </si>
-  <si>
-    <t>CHEM1041</t>
-  </si>
-  <si>
-    <t>CHEM1046</t>
-  </si>
-  <si>
-    <t>CHEM1072</t>
-  </si>
-  <si>
-    <t>CHEM1077</t>
-  </si>
-  <si>
-    <t>CHEM2401</t>
-  </si>
-  <si>
-    <t>CLAS1403</t>
-  </si>
-  <si>
-    <t>CLAS1413</t>
-  </si>
-  <si>
-    <t>CLAS1503</t>
-  </si>
-  <si>
-    <t>CLAS3053</t>
-  </si>
-  <si>
-    <t>CS1003</t>
-  </si>
-  <si>
-    <t>CS1023</t>
-  </si>
-  <si>
-    <t>ECON1001</t>
-  </si>
-  <si>
-    <t>ECON1013</t>
-  </si>
-  <si>
-    <t>ECON1023</t>
-  </si>
-  <si>
-    <t>ECON1073</t>
-  </si>
-  <si>
-    <t>ENGG1003</t>
-  </si>
-  <si>
-    <t>ENGG1015</t>
-  </si>
-  <si>
-    <t>ENGG1082</t>
-  </si>
-  <si>
-    <t>ENGG4013</t>
-  </si>
-  <si>
-    <t>FR1304</t>
-  </si>
-  <si>
-    <t>GEOL1001</t>
-  </si>
-  <si>
-    <t>GEOL1044</t>
-  </si>
-  <si>
-    <t>GEOL1063</t>
-  </si>
-  <si>
-    <t>GEOL1074</t>
-  </si>
-  <si>
-    <t>GER1001</t>
-  </si>
-  <si>
-    <t>GER4023</t>
-  </si>
-  <si>
-    <t>HIST1001</t>
-  </si>
-  <si>
-    <t>HIST3414</t>
-  </si>
-  <si>
-    <t>HIST3925</t>
-  </si>
-  <si>
-    <t>HIST3975</t>
-  </si>
-  <si>
-    <t>HUM1401</t>
-  </si>
-  <si>
-    <t>JPNS1013</t>
-  </si>
-  <si>
-    <t>MATH1003</t>
-  </si>
-  <si>
-    <t>MATH1013</t>
-  </si>
-  <si>
-    <t>MATH1503</t>
-  </si>
-  <si>
-    <t>MATH2513</t>
-  </si>
-  <si>
-    <t>MATH3503</t>
-  </si>
-  <si>
-    <t>PHIL1053</t>
-  </si>
-  <si>
-    <t>PHIL1101</t>
-  </si>
-  <si>
-    <t>PHYS5993</t>
-  </si>
-  <si>
-    <t>POLS1201</t>
-  </si>
-  <si>
-    <t>POLS1203</t>
-  </si>
-  <si>
-    <t>POLS1301</t>
-  </si>
-  <si>
-    <t>POLS1603</t>
-  </si>
-  <si>
-    <t>PSYC1003</t>
-  </si>
-  <si>
-    <t>PSYC1013</t>
-  </si>
-  <si>
-    <t>PSYC1023</t>
-  </si>
-  <si>
-    <t>RCLP1042</t>
-  </si>
-  <si>
-    <t>RUSS1013</t>
-  </si>
-  <si>
-    <t>SE1001</t>
-  </si>
-  <si>
-    <t>SEP1001</t>
-  </si>
-  <si>
-    <t>SOCI1001</t>
-  </si>
-  <si>
-    <t>SOCI1503</t>
-  </si>
-  <si>
-    <t>SOCI1523</t>
-  </si>
-  <si>
-    <t>SOCI1583</t>
-  </si>
-  <si>
-    <t>SOCI2533</t>
-  </si>
-  <si>
-    <t>SOCI2534</t>
-  </si>
-  <si>
-    <t>SPAN1203</t>
-  </si>
-  <si>
-    <t>STAT2593</t>
-  </si>
-  <si>
-    <t>STS1003</t>
-  </si>
-  <si>
-    <t>TME1001</t>
-  </si>
-  <si>
-    <t>TME3013</t>
-  </si>
-  <si>
-    <t>TME3113</t>
-  </si>
-  <si>
-    <t>TME3213</t>
-  </si>
-  <si>
-    <t>TME3313</t>
-  </si>
-  <si>
-    <t>TME3346</t>
-  </si>
-  <si>
-    <t>TME3413</t>
-  </si>
-  <si>
-    <t>TME5025</t>
-  </si>
-  <si>
-    <t>WLCS1002</t>
-  </si>
-  <si>
-    <t>MATH</t>
-  </si>
-  <si>
-    <t>SCIENCE</t>
-  </si>
-  <si>
-    <t>FUNDAMENTALS</t>
-  </si>
-  <si>
-    <t>SPECIALIZED</t>
-  </si>
-  <si>
-    <t>TERMINAL</t>
-  </si>
-  <si>
-    <t>CORE</t>
-  </si>
-  <si>
-    <t>CSE</t>
-  </si>
-  <si>
-    <t>AESL1011</t>
-  </si>
-  <si>
-    <t>CHE2501</t>
-  </si>
-  <si>
-    <t>CHE2506</t>
-  </si>
-  <si>
-    <t>CS1073</t>
-  </si>
-  <si>
-    <t>CS1083</t>
-  </si>
-  <si>
-    <t>CS1203</t>
-  </si>
-  <si>
-    <t>CS3383</t>
-  </si>
-  <si>
-    <t>CS3413</t>
-  </si>
-  <si>
-    <t>CS3853</t>
-  </si>
-  <si>
-    <t>CS6895</t>
-  </si>
-  <si>
-    <t>ECE4143</t>
-  </si>
-  <si>
-    <t>ECE4253</t>
-  </si>
-  <si>
-    <t>ECE4261</t>
-  </si>
-  <si>
-    <t>ECE4323</t>
-  </si>
-  <si>
-    <t>ECE4333</t>
-  </si>
-  <si>
-    <t>ECE4923</t>
-  </si>
-  <si>
-    <t>ECE4933</t>
-  </si>
-  <si>
-    <t>EE6013</t>
-  </si>
-  <si>
-    <t>EE6463</t>
-  </si>
-  <si>
-    <t>EE6513</t>
-  </si>
-  <si>
-    <t>EE6603</t>
-  </si>
-  <si>
-    <t>EE6653</t>
-  </si>
-  <si>
-    <t>EE6997</t>
-  </si>
-  <si>
-    <t>ENGG1001</t>
-  </si>
-  <si>
-    <t>ENGG1013</t>
-  </si>
-  <si>
-    <t>ENGL1500</t>
-  </si>
-  <si>
-    <t>ENVS2023</t>
-  </si>
-  <si>
-    <t>ESCI1012</t>
-  </si>
-  <si>
-    <t>ESL1301</t>
-  </si>
-  <si>
-    <t>ESL1302</t>
-  </si>
-  <si>
-    <t>ESL1303</t>
-  </si>
-  <si>
-    <t>KIN2603</t>
-  </si>
-  <si>
-    <t>KIN3061</t>
-  </si>
-  <si>
-    <t>MAAC3065</t>
-  </si>
-  <si>
-    <t>MATH0863</t>
-  </si>
-  <si>
-    <t>MATH1053</t>
-  </si>
-  <si>
-    <t>MATH1063</t>
-  </si>
-  <si>
-    <t>MATH1863</t>
-  </si>
-  <si>
-    <t>MATH2903</t>
-  </si>
-  <si>
-    <t>MATH3003</t>
-  </si>
-  <si>
-    <t>MATH3213</t>
-  </si>
-  <si>
-    <t>MATH3243</t>
-  </si>
-  <si>
-    <t>MATH3343</t>
-  </si>
-  <si>
-    <t>MATH3543</t>
-  </si>
-  <si>
-    <t>ME1312</t>
-  </si>
-  <si>
-    <t>ME2111</t>
-  </si>
-  <si>
-    <t>ME2122</t>
-  </si>
-  <si>
-    <t>ME2125</t>
-  </si>
-  <si>
-    <t>ME2143</t>
-  </si>
-  <si>
-    <t>ME2145</t>
-  </si>
-  <si>
-    <t>ME3413</t>
-  </si>
-  <si>
-    <t>ME3415</t>
-  </si>
-  <si>
-    <t>PHYS1000</t>
-  </si>
-  <si>
-    <t>PHYS1081</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>SOCIETY</t>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>MATH3373</t>
   </si>
 </sst>
 </file>
@@ -1141,12 +1028,12 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1166,9 +1053,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1186,9 +1073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1206,9 +1093,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1226,9 +1113,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1246,9 +1133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1266,9 +1153,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1286,9 +1173,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1306,9 +1193,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1326,9 +1213,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1346,9 +1233,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1366,9 +1253,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1386,9 +1273,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1406,9 +1293,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1426,9 +1313,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1446,9 +1333,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1466,9 +1353,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1486,9 +1373,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1506,9 +1393,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1526,9 +1413,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>56</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1546,9 +1433,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1566,9 +1453,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1586,9 +1473,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1606,9 +1493,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1626,9 +1513,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1646,9 +1533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -1666,9 +1553,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1686,9 +1573,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -1706,9 +1593,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -1726,9 +1613,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -1746,9 +1633,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -1766,9 +1653,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -1786,9 +1673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1806,9 +1693,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1826,9 +1713,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1846,9 +1733,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1866,9 +1753,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1886,9 +1773,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1906,9 +1793,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1926,9 +1813,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1946,9 +1833,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -1966,9 +1853,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1986,9 +1873,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2006,9 +1893,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2026,9 +1913,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2046,9 +1933,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -2066,9 +1953,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -2086,9 +1973,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -2106,9 +1993,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -2126,9 +2013,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2146,9 +2033,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -2166,9 +2053,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -2186,9 +2073,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -2206,9 +2093,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -2226,9 +2113,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -2246,9 +2133,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -2266,9 +2153,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -2286,9 +2173,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -2306,9 +2193,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2326,9 +2213,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -2346,9 +2233,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -2366,9 +2253,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -2386,9 +2273,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -2406,9 +2293,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -2426,9 +2313,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -2446,9 +2333,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -2466,9 +2353,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2486,9 +2373,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2506,9 +2393,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2526,9 +2413,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -2546,9 +2433,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -2566,9 +2453,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -2586,9 +2473,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B73">
         <v>29</v>
@@ -2606,9 +2493,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -2626,9 +2513,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -2646,9 +2533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2666,9 +2553,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -2686,9 +2573,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2706,9 +2593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -2726,9 +2613,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -2746,9 +2633,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>202</v>
+        <v>159</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -2766,9 +2653,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2786,9 +2673,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -2806,9 +2693,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -2826,9 +2713,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -2846,9 +2733,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -2866,9 +2753,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -2886,9 +2773,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -2906,9 +2793,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -2926,9 +2813,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -2946,9 +2833,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2966,9 +2853,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B92">
         <v>49</v>
@@ -2986,9 +2873,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -3006,9 +2893,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -3026,9 +2913,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -3046,9 +2933,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -3066,9 +2953,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -3086,9 +2973,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -3106,9 +2993,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -3126,9 +3013,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -3146,9 +3033,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -3166,9 +3053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -3186,9 +3073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="B103">
         <v>15</v>
@@ -3206,9 +3093,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -3226,9 +3113,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -3246,9 +3133,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -3266,9 +3153,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -3286,9 +3173,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -3306,9 +3193,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -3326,9 +3213,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -3346,9 +3233,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -3366,9 +3253,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="B112">
         <v>2</v>
@@ -3386,9 +3273,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -3406,9 +3293,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -3426,9 +3313,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -3446,9 +3333,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -3466,9 +3353,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -3486,9 +3373,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -3506,9 +3393,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -3526,9 +3413,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -3546,9 +3433,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -3566,9 +3453,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -3586,9 +3473,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -3606,9 +3493,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -3626,9 +3513,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="B125">
         <v>4</v>
@@ -3646,9 +3533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -3666,9 +3553,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -3686,9 +3573,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>219</v>
+        <v>176</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -3706,9 +3593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -3726,9 +3613,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -3746,9 +3633,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -3766,9 +3653,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="B132">
         <v>2</v>
@@ -3786,9 +3673,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="B133">
         <v>2</v>
@@ -3806,9 +3693,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -3826,9 +3713,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -3846,9 +3733,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -3866,9 +3753,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -3886,9 +3773,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -3906,9 +3793,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -3926,9 +3813,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="B140">
         <v>3</v>
@@ -3946,9 +3833,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>228</v>
+        <v>185</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -3966,9 +3853,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="B142">
         <v>3</v>
@@ -3986,9 +3873,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>230</v>
+        <v>187</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -4006,9 +3893,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -4026,9 +3913,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>231</v>
+        <v>188</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -4046,9 +3933,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -4066,9 +3953,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -4086,9 +3973,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -4106,9 +3993,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -4126,9 +4013,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -4146,9 +4033,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -4166,9 +4053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -4186,9 +4073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -4206,9 +4093,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -4226,9 +4113,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -4246,9 +4133,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -4266,9 +4153,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -4286,9 +4173,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -4306,9 +4193,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -4326,9 +4213,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -4346,9 +4233,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -4366,9 +4253,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -4386,9 +4273,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -4406,9 +4293,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -4426,9 +4313,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -4446,9 +4333,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -4466,9 +4353,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -4486,9 +4373,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -4506,9 +4393,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -4526,9 +4413,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="B170">
         <v>3</v>
@@ -4546,9 +4433,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -4566,9 +4453,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -4586,9 +4473,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -4606,9 +4493,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -4626,9 +4513,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -4646,9 +4533,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -4666,9 +4553,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -4686,9 +4573,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -4706,9 +4593,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -4726,9 +4613,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -4746,9 +4633,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -4766,9 +4653,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -4786,9 +4673,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -4806,9 +4693,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -4826,9 +4713,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -4846,9 +4733,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="B186">
         <v>3</v>
@@ -4866,9 +4753,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -4895,15 +4782,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -4921,9 +4808,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4941,9 +4828,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4961,9 +4848,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4981,9 +4868,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5001,9 +4888,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -5021,9 +4908,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -5041,9 +4928,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5061,9 +4948,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -5088,248 +4975,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="K1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:AH5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K2" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" t="s">
-        <v>43</v>
-      </c>
-      <c r="S2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" t="s">
-        <v>55</v>
-      </c>
-      <c r="X2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" t="s">
-        <v>65</v>
-      </c>
-      <c r="V3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="V4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -5339,655 +5006,80 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>105</v>
       </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>135</v>
-      </c>
-      <c r="F26" t="s">
-        <v>127</v>
-      </c>
-      <c r="G26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>129</v>
-      </c>
-      <c r="G28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
-        <v>147</v>
-      </c>
-      <c r="G33" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>170</v>
-      </c>
-      <c r="G35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>175</v>
-      </c>
-      <c r="G36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G38" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G58" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G59" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G60" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G61" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G62" t="s">
-        <v>180</v>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Area distribution with console output; Excel output to come soon (3rd time's the charm...)
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\test\test - Copy (3)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Uni\SWE 2043\Application\Team6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE830D2-00D8-40B1-B947-C840516C4AC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228624C-09BB-4099-B91F-6822394B7197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3315" windowWidth="16860" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3768" yWindow="3312" windowWidth="16860" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equivelents" sheetId="2" r:id="rId1"/>
@@ -956,13 +956,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:AH5"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>74</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="V4" t="s">
         <v>62</v>
       </c>
@@ -1207,19 +1207,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>98</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>99</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>100</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>102</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>103</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>104</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>105</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>106</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>107</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>108</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>109</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>126</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>127</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>128</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>129</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>145</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>123</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
         <v>124</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F30" t="s">
         <v>138</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F31" t="s">
         <v>139</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
         <v>140</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>141</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
         <v>142</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
         <v>164</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36" t="s">
         <v>169</v>
       </c>
@@ -1726,132 +1726,132 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G38" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G39" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G40" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G41" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G44" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G47" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
       <c r="G48" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G49" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G50" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G52" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G53" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G54" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G55" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G56" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G58" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G59" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G60" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G61" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G62" t="s">
         <v>174</v>
       </c>

</xml_diff>

<commit_message>
trying to read config file.
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Uni\SWE 2043\Application\Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uwesh/Desktop/Team6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228624C-09BB-4099-B91F-6822394B7197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B1768D-F391-B945-8AE1-554B0508F396}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3768" yWindow="3312" windowWidth="16860" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3760" yWindow="3320" windowWidth="16860" windowHeight="11380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equivelents" sheetId="2" r:id="rId1"/>
     <sheet name="Areas" sheetId="3" r:id="rId2"/>
+    <sheet name="GLOBAL DIST." sheetId="4" r:id="rId3"/>
+    <sheet name="RAW" sheetId="5" r:id="rId4"/>
+    <sheet name="MASTERLIST" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
@@ -953,16 +956,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC837E03-0573-934B-B24D-6758F5CE55AD}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>74</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="V4" t="s">
         <v>62</v>
       </c>
@@ -1204,22 +1207,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBC0823-DDE6-2341-B765-3A4A4B37569E}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1323,7 +1326,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>98</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>99</v>
       </c>
@@ -1432,7 +1435,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>100</v>
       </c>
@@ -1446,7 +1449,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>102</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>103</v>
       </c>
@@ -1488,7 +1491,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>104</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>105</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>106</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>107</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>108</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>109</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>126</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>127</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>128</v>
       </c>
@@ -1632,7 +1635,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>129</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>145</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F28" t="s">
         <v>123</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>124</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
         <v>138</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
         <v>139</v>
       </c>
@@ -1686,7 +1689,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
         <v>140</v>
       </c>
@@ -1694,7 +1697,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F33" t="s">
         <v>141</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F34" t="s">
         <v>142</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
         <v>164</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F36" t="s">
         <v>169</v>
       </c>
@@ -1726,132 +1729,132 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G38" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G39" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G40" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G41" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G44" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G47" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G48" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G49" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G50" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G51" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G52" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G53" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G54" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G55" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G56" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G58" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G59" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G60" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G61" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G62" t="s">
         <v>174</v>
       </c>
@@ -1859,4 +1862,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD990CA0-5D4D-204B-BAFA-7380DA109DD6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="A1:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383F74F1-3A0F-284C-B93A-FD7F5356AEC3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G128"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6486BBAF-285C-0745-AEFD-DCAC364B021F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A154"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel file input dialog window, now only shows .xlsx
</commit_message>
<xml_diff>
--- a/results_EE2014.xlsx
+++ b/results_EE2014.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Uni\SWE 2043\Application\Team6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F228624C-09BB-4099-B91F-6822394B7197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9774271F-2999-4A85-A943-A875341496A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3768" yWindow="3312" windowWidth="16860" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4275" windowWidth="23205" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equivelents" sheetId="2" r:id="rId1"/>
@@ -953,16 +953,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F717F1-DAE4-4F68-A6A0-C36614B50A31}">
   <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+      <selection sqref="A1:AH5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>74</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="V4" t="s">
         <v>62</v>
       </c>
@@ -1204,22 +1204,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D1D2E9-E343-4F94-B2B3-6B8F6D403AA4}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>98</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>99</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>100</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>101</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>102</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>103</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>104</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>105</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>106</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>107</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>108</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>109</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>67</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>68</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>110</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>126</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>127</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>128</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>129</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>145</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>123</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>124</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>138</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>139</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>140</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
         <v>141</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>142</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>164</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>169</v>
       </c>
@@ -1726,132 +1726,132 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:7" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>174</v>
       </c>

</xml_diff>